<commit_message>
added bbtools script and undated paired end read targets
</commit_message>
<xml_diff>
--- a/targets_PE.xlsx
+++ b/targets_PE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="2100" windowWidth="24060" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="4800" windowWidth="28620" windowHeight="13960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="317">
   <si>
     <t>SampleName</t>
   </si>
@@ -312,309 +312,9 @@
     <t>SRR5043899</t>
   </si>
   <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/ERR498201_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/ERR498201_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR526975_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334340_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334339_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334212_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334213_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334214_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334215_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334216_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334217_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334218_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334219_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334220_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334221_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR497890_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR497891_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR623231_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR960386_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR826503_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR957603_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR1060328_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR967068_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601482_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601571_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601666_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601689_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601690_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601692_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601694_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601695_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601696_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601698_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601699_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601701_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601702_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601703_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601704_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601705_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601706_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601707_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601709_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601711_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601712_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601714_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601716_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601718_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043896_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043897_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043898_1.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043899_1.fastq</t>
-  </si>
-  <si>
     <t>## 52</t>
   </si>
   <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR526975_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334340_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334339_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334212_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334213_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334214_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334215_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334216_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334217_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334218_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334219_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334220_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR334221_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR497890_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR497891_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR623231_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR960386_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR826503_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR957603_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR1060328_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR967068_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601482_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601571_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601666_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601689_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601690_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601692_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601694_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601695_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601696_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601698_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601699_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601701_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601702_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601703_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601704_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601705_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601706_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601707_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601709_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601711_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601712_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601714_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601716_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR2601718_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043896_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043897_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043898_2.fastq</t>
-  </si>
-  <si>
-    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/SRR5043899_2.fastq</t>
-  </si>
-  <si>
     <t>BioProjectAcc</t>
   </si>
   <si>
@@ -936,9 +636,6 @@
     <t>## [6]</t>
   </si>
   <si>
-    <t>"# &lt;CMP&gt; CMPset4:</t>
-  </si>
-  <si>
     <t>"#Project file for Paired End SRA targets for C_gigas under different stress conditions"</t>
   </si>
   <si>
@@ -967,6 +664,312 @@
   </si>
   <si>
     <t>## 58</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043899_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043898_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043897_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043896_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601718_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601716_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601714_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601712_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601711_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601709_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601707_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601706_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601705_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601704_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601703_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601702_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601701_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601699_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601698_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601696_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601695_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601694_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601692_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601690_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601689_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601666_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601571_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601482_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_ERR498201_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR967068_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR1060328_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR957603_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR826503_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR960386_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR623231_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR497891_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR497890_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR526975_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334340_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334339_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334221_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334220_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334219_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334218_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334217_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334216_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334215_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334214_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334213_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334212_1.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043899_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043898_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043897_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR5043896_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601718_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601716_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601714_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601712_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601711_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601709_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601707_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601706_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601705_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601704_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601703_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601702_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601701_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601699_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601698_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601696_2.fastq</t>
+  </si>
+  <si>
+    <t>FileName1</t>
+  </si>
+  <si>
+    <t>FileName2</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601695_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601694_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601692_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601690_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601689_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601666_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601571_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR2601482_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_ERR498201_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR967068_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR1060328_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR957603_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR826503_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR960386_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR623231_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR497891_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR497890_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR526975_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334340_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334339_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334221_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334220_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334219_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334218_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334217_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334216_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334215_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334214_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334213_2.fastq</t>
+  </si>
+  <si>
+    <t>/data3/marine_diseases_lab/erin/Bio_project_SRA/quality_trim_and_filtered_SRR334212_2.fastq</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1055,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1071,6 +1074,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
@@ -1091,7 +1096,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1101,6 +1106,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1441,14 +1448,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A26"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="75.83203125" customWidth="1"/>
-    <col min="3" max="3" width="64.83203125" customWidth="1"/>
+    <col min="2" max="2" width="94" customWidth="1"/>
+    <col min="3" max="3" width="92" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
@@ -1458,62 +1465,65 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>198</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>306</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>199</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>201</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>307</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>308</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>309</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>304</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>285</v>
       </c>
       <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>198</v>
+      <c r="G6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1521,22 +1531,22 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>247</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>96</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1544,22 +1554,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>196</v>
+        <v>266</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>201</v>
+        <v>101</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>248</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1567,22 +1577,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>195</v>
+        <v>267</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>202</v>
+        <v>102</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>249</v>
+        <v>149</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1590,22 +1600,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>144</v>
+        <v>218</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>194</v>
+        <v>268</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1613,22 +1623,22 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>193</v>
+        <v>269</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>251</v>
+        <v>151</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1636,22 +1646,22 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>220</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>192</v>
+        <v>270</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>252</v>
+        <v>152</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>91</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1659,22 +1669,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>221</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>191</v>
+        <v>271</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>207</v>
+        <v>107</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>253</v>
+        <v>153</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>90</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1682,22 +1692,22 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>190</v>
+        <v>272</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>208</v>
+        <v>108</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>254</v>
+        <v>154</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>89</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1705,22 +1715,22 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>209</v>
+        <v>109</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1728,22 +1738,22 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>188</v>
+        <v>274</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>256</v>
+        <v>156</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>87</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1751,22 +1761,22 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>187</v>
+        <v>275</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>257</v>
+        <v>157</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>86</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1774,22 +1784,22 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>136</v>
+        <v>226</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>211</v>
+        <v>111</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>258</v>
+        <v>158</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>85</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1797,22 +1807,22 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>185</v>
+        <v>277</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>212</v>
+        <v>112</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>259</v>
+        <v>159</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>84</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1820,22 +1830,22 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>184</v>
+        <v>278</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>260</v>
+        <v>160</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>83</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1843,22 +1853,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>229</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>214</v>
+        <v>114</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>261</v>
+        <v>161</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>82</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1866,22 +1876,22 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>132</v>
+        <v>230</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>182</v>
+        <v>280</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>262</v>
+        <v>162</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1889,22 +1899,22 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>231</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>181</v>
+        <v>281</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>214</v>
+        <v>114</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>263</v>
+        <v>163</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>80</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1912,22 +1922,22 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>180</v>
+        <v>282</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>209</v>
+        <v>109</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>264</v>
+        <v>164</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1935,22 +1945,22 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>179</v>
+        <v>283</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>265</v>
+        <v>165</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1958,22 +1968,22 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>266</v>
+        <v>166</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>77</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1981,22 +1991,22 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>177</v>
+        <v>287</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>212</v>
+        <v>112</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>267</v>
+        <v>167</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2004,22 +2014,22 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>176</v>
+        <v>288</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>268</v>
+        <v>168</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>75</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2027,22 +2037,22 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>125</v>
+        <v>237</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>175</v>
+        <v>289</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>269</v>
+        <v>169</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>74</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2050,22 +2060,22 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>174</v>
+        <v>290</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>208</v>
+        <v>108</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2073,22 +2083,22 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>123</v>
+        <v>239</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>211</v>
+        <v>111</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>271</v>
+        <v>171</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2096,22 +2106,22 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>272</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2119,22 +2129,22 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>121</v>
+        <v>241</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>171</v>
+        <v>293</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>273</v>
+        <v>173</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>70</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2142,22 +2152,22 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>120</v>
+        <v>242</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>170</v>
+        <v>294</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>207</v>
+        <v>107</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>274</v>
+        <v>174</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>69</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16">
@@ -2165,22 +2175,22 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>97</v>
+        <v>243</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>217</v>
+        <v>117</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>275</v>
+        <v>175</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>47</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>218</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16">
@@ -2188,22 +2198,22 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>119</v>
+        <v>244</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>169</v>
+        <v>296</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>276</v>
+        <v>176</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>219</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2211,22 +2221,22 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>245</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>168</v>
+        <v>297</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>221</v>
+        <v>121</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>277</v>
+        <v>177</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>67</v>
       </c>
       <c r="G37" t="s">
-        <v>222</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2234,22 +2244,22 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>246</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>167</v>
+        <v>298</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>223</v>
+        <v>123</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>278</v>
+        <v>178</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16">
@@ -2257,22 +2267,22 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>225</v>
+        <v>125</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>279</v>
+        <v>179</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>226</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16">
@@ -2280,22 +2290,22 @@
         <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>115</v>
+        <v>248</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>165</v>
+        <v>300</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>227</v>
+        <v>127</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>280</v>
+        <v>180</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>228</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16">
@@ -2303,22 +2313,22 @@
         <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>249</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>164</v>
+        <v>301</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>229</v>
+        <v>129</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>281</v>
+        <v>181</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>230</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16">
@@ -2326,22 +2336,22 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>114</v>
+        <v>249</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>164</v>
+        <v>301</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>229</v>
+        <v>129</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>282</v>
+        <v>182</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="16">
@@ -2349,22 +2359,22 @@
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>113</v>
+        <v>250</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>302</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>283</v>
+        <v>183</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>62</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>233</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="16">
@@ -2372,22 +2382,22 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>112</v>
+        <v>251</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>162</v>
+        <v>303</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>284</v>
+        <v>184</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>233</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="16">
@@ -2395,22 +2405,22 @@
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>149</v>
+        <v>304</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>234</v>
+        <v>134</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>285</v>
+        <v>185</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>48</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16">
@@ -2418,22 +2428,22 @@
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>150</v>
+        <v>305</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>236</v>
+        <v>136</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>286</v>
+        <v>186</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>49</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="16">
@@ -2441,22 +2451,22 @@
         <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>101</v>
+        <v>254</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>151</v>
+        <v>306</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>237</v>
+        <v>137</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>287</v>
+        <v>187</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="16">
@@ -2464,22 +2474,22 @@
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>255</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>161</v>
+        <v>307</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>238</v>
+        <v>138</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>288</v>
+        <v>188</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>60</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="16">
@@ -2487,22 +2497,22 @@
         <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>110</v>
+        <v>256</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>160</v>
+        <v>308</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>239</v>
+        <v>139</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>289</v>
+        <v>189</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>59</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="16">
@@ -2510,183 +2520,183 @@
         <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>257</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>159</v>
+        <v>309</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>240</v>
+        <v>140</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="16">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>158</v>
+        <v>310</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>241</v>
+        <v>141</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>291</v>
+        <v>191</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>57</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="16">
       <c r="A52" t="s">
-        <v>310</v>
+        <v>209</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>107</v>
+        <v>259</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>157</v>
+        <v>311</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>242</v>
+        <v>142</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>292</v>
+        <v>192</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>56</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="16">
       <c r="A53" t="s">
-        <v>311</v>
+        <v>210</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>106</v>
+        <v>260</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>156</v>
+        <v>312</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>243</v>
+        <v>143</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>293</v>
+        <v>193</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>55</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="16">
       <c r="A54" t="s">
-        <v>312</v>
+        <v>211</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>105</v>
+        <v>261</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>155</v>
+        <v>313</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>244</v>
+        <v>144</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>294</v>
+        <v>194</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="16">
       <c r="A55" t="s">
-        <v>313</v>
+        <v>212</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>104</v>
+        <v>262</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>154</v>
+        <v>314</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>238</v>
+        <v>138</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>295</v>
+        <v>195</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>53</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="16">
       <c r="A56" t="s">
-        <v>314</v>
+        <v>213</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>153</v>
+        <v>315</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>245</v>
+        <v>145</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>296</v>
+        <v>196</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>52</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="16">
       <c r="A57" t="s">
-        <v>315</v>
+        <v>214</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>102</v>
+        <v>264</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>246</v>
+        <v>146</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>